<commit_message>
Enhancement: Improved DOM and iframe element detection and filling - prioritize iframe searching, add case-insensitive matching, better element identification
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -463,25 +463,25 @@
         <v>Login functionality with valid and invalid credentials</v>
       </c>
       <c r="D2" t="str">
-        <v>TS001BR001</v>
+        <v>TS001TC001</v>
       </c>
       <c r="E2" t="str">
         <v>Verify the url is opened</v>
       </c>
       <c r="F2" t="str">
-        <v>TS001TC001BR001</v>
+        <v>TS001TC001TSP001</v>
       </c>
       <c r="G2" t="str">
-        <v xml:space="preserve">Open BR.NET url </v>
+        <v xml:space="preserve">Open ORACLE url </v>
       </c>
       <c r="H2" t="str">
         <v>OPEN_URL</v>
       </c>
       <c r="I2" t="str">
-        <v>https://iblbcuat.indusind.com/IndusindUAT.html</v>
+        <v>https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
       </c>
       <c r="J2" t="str">
-        <v>https://iblbcuat.indusind.com/IndusindUAT.html</v>
+        <v>https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
       </c>
       <c r="K2" t="str">
         <v xml:space="preserve">URL is opened </v>
@@ -493,7 +493,7 @@
         <v/>
       </c>
       <c r="N2" t="str">
-        <v>Opened: https://iblbcuat.indusind.com/IndusindUAT.html</v>
+        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
       </c>
       <c r="O2" t="str">
         <v>screenshots/STEP_1.png</v>
@@ -504,48 +504,39 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F3" t="str">
-        <v>TS001TC001BR002</v>
+        <v>TS001TC001TSP002</v>
       </c>
       <c r="G3" t="str">
-        <v>enter username</v>
+        <v>enter userid</v>
       </c>
       <c r="H3" t="str">
         <v>fill</v>
       </c>
       <c r="I3" t="str">
-        <v>Enter User Name</v>
+        <v>USER ID</v>
       </c>
       <c r="J3" t="str">
-        <v>SINDU</v>
+        <v>SAI_MAK</v>
       </c>
       <c r="K3" t="str">
         <v>username should be entered</v>
       </c>
       <c r="L3" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M3" t="str">
-        <v/>
-      </c>
-      <c r="N3" t="str">
-        <v>Filled: Enter User Name</v>
-      </c>
-      <c r="O3" t="str">
-        <v>screenshots/STEP_2.png</v>
-      </c>
-      <c r="P3" t="str">
-        <v>page_sources/STEP_2_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F4" t="str">
-        <v>TS001TC001BR003</v>
+        <v>TS001TC001TSP003</v>
       </c>
       <c r="G4" t="str">
         <v>Enter Password</v>
@@ -554,118 +545,112 @@
         <v>fill</v>
       </c>
       <c r="I4" t="str">
-        <v>Enter Password</v>
+        <v>Password</v>
       </c>
       <c r="J4" t="str">
-        <v>Test@123</v>
+        <v>Pranitha@25</v>
       </c>
       <c r="K4" t="str">
         <v>password should be entered</v>
       </c>
       <c r="L4" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
-        <v>Filled: Enter Password</v>
-      </c>
-      <c r="O4" t="str">
-        <v>screenshots/STEP_3.png</v>
-      </c>
-      <c r="P4" t="str">
-        <v>page_sources/STEP_3_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F5" t="str">
-        <v>TS001TC001BR004</v>
+        <v>TS001TC001TSP004</v>
       </c>
       <c r="G5" t="str">
-        <v xml:space="preserve">Click login </v>
+        <v xml:space="preserve">Click Signin </v>
       </c>
       <c r="H5" t="str">
         <v>click</v>
       </c>
       <c r="I5" t="str">
-        <v>Login</v>
+        <v>Sign In</v>
       </c>
       <c r="K5" t="str">
-        <v>Login in button should be clicked</v>
+        <v>Sign in button should be clicked</v>
       </c>
       <c r="L5" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
-        <v>Clicked: Login</v>
-      </c>
-      <c r="O5" t="str">
-        <v>screenshots/STEP_4.png</v>
-      </c>
-      <c r="P5" t="str">
-        <v>page_sources/STEP_4_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F6" t="str">
-        <v>TS001TC001BR005</v>
+        <v>TS001TC001TSP005</v>
       </c>
       <c r="G6" t="str">
-        <v xml:space="preserve">Click Start </v>
+        <v xml:space="preserve">Click OK button of the information message popup window </v>
       </c>
       <c r="H6" t="str">
         <v>click</v>
       </c>
       <c r="I6" t="str">
-        <v>Click To Open</v>
-      </c>
-      <c r="K6" t="str">
-        <v>Start button should be clicked</v>
+        <v>Ok</v>
       </c>
       <c r="L6" t="str">
-        <v>FAIL</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M6" t="str">
-        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
-      </c>
-      <c r="N6" t="str">
-        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
-      </c>
-      <c r="O6" t="str">
-        <v/>
-      </c>
-      <c r="P6" t="str">
-        <v/>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>YES</v>
       </c>
+      <c r="D7" t="str">
+        <v>TS001TC002</v>
+      </c>
+      <c r="E7" t="str">
+        <v>STDCIF creation</v>
+      </c>
       <c r="F7" t="str">
-        <v>TS001TC001BR006</v>
+        <v>TS001TC002TSP001</v>
       </c>
       <c r="G7" t="str">
-        <v>Click Change Branch</v>
+        <v>Enter STDCIF in the Function Id</v>
       </c>
       <c r="H7" t="str">
-        <v>click</v>
+        <v>fill</v>
       </c>
       <c r="I7" t="str">
-        <v>Change Branch</v>
+        <v>Function Id</v>
+      </c>
+      <c r="J7" t="str">
+        <v>STDCIF</v>
       </c>
       <c r="K7" t="str">
-        <v xml:space="preserve"> Change Branch be clicked</v>
+        <v>Fucntion Id should be filled with STDCIF</v>
+      </c>
+      <c r="L7" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v>Filled: Function Id</v>
+      </c>
+      <c r="O7" t="str">
+        <v>screenshots/STEP_6.png</v>
+      </c>
+      <c r="P7" t="str">
+        <v>page_sources/STEP_6_source.html</v>
       </c>
     </row>
     <row r="8">
@@ -673,22 +658,34 @@
         <v>YES</v>
       </c>
       <c r="F8" t="str">
-        <v>TS001TC001BR008</v>
+        <v>TS001TC002TSP002</v>
       </c>
       <c r="G8" t="str">
-        <v>Enter Branch ID</v>
+        <v>Click the Go button</v>
       </c>
       <c r="H8" t="str">
-        <v>fill</v>
+        <v>click</v>
       </c>
       <c r="I8" t="str">
-        <v>Branch ID</v>
-      </c>
-      <c r="J8">
-        <v>200064</v>
+        <v>Go</v>
       </c>
       <c r="K8" t="str">
-        <v>Branch ID should be entered</v>
+        <v xml:space="preserve">GO button should be clicked </v>
+      </c>
+      <c r="L8" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v>Clicked: Go</v>
+      </c>
+      <c r="O8" t="str">
+        <v>screenshots/STEP_7.png</v>
+      </c>
+      <c r="P8" t="str">
+        <v>page_sources/STEP_7_source.html</v>
       </c>
     </row>
     <row r="9">
@@ -696,19 +693,34 @@
         <v>YES</v>
       </c>
       <c r="F9" t="str">
-        <v>TS001TC001BR008</v>
+        <v>TS001TC002TSP003</v>
       </c>
       <c r="G9" t="str">
-        <v>Click Ok</v>
+        <v xml:space="preserve">Click Enter Query </v>
       </c>
       <c r="H9" t="str">
         <v>click</v>
       </c>
       <c r="I9" t="str">
-        <v>Ok</v>
+        <v>Enter Query</v>
       </c>
       <c r="K9" t="str">
-        <v>Ok should be entered</v>
+        <v xml:space="preserve">New should be clicked </v>
+      </c>
+      <c r="L9" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M9" t="str">
+        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+      </c>
+      <c r="N9" t="str">
+        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -716,19 +728,19 @@
         <v>YES</v>
       </c>
       <c r="F10" t="str">
-        <v>TS001TC001BR009</v>
+        <v>TS001TC002TSP004</v>
       </c>
       <c r="G10" t="str">
-        <v xml:space="preserve">Click Start </v>
+        <v>On the customer No. field Click on "P" to generate customer no</v>
       </c>
       <c r="H10" t="str">
         <v>click</v>
       </c>
       <c r="I10" t="str">
-        <v>Click To Open</v>
+        <v>P</v>
       </c>
       <c r="K10" t="str">
-        <v>Start button should be clicked</v>
+        <v>P should be clicked and Customer No should be generated</v>
       </c>
     </row>
     <row r="11">
@@ -736,19 +748,22 @@
         <v>YES</v>
       </c>
       <c r="F11" t="str">
-        <v>TS001TC001BR010</v>
+        <v>TS001TC002TSP005</v>
       </c>
       <c r="G11" t="str">
-        <v>Click Advance &amp; Collateral</v>
+        <v xml:space="preserve">enter full name </v>
       </c>
       <c r="H11" t="str">
-        <v>click</v>
+        <v>fill</v>
       </c>
       <c r="I11" t="str">
-        <v>Advance &amp; Collateral</v>
+        <v>Full Name</v>
+      </c>
+      <c r="J11" t="str">
+        <v>AUTO24</v>
       </c>
       <c r="K11" t="str">
-        <v>Advance &amp; Collateralshould be clicked</v>
+        <v xml:space="preserve">First name should be filled </v>
       </c>
     </row>
     <row r="12">
@@ -756,19 +771,22 @@
         <v>YES</v>
       </c>
       <c r="F12" t="str">
-        <v>TS001TC001BR011</v>
+        <v>TS001TC002TSP006</v>
       </c>
       <c r="G12" t="str">
-        <v>Click Loan Maintenance</v>
+        <v>enter short name</v>
       </c>
       <c r="H12" t="str">
-        <v>click</v>
+        <v>fill</v>
       </c>
       <c r="I12" t="str">
-        <v>Loan Maintenance</v>
+        <v>Short Name</v>
+      </c>
+      <c r="J12" t="str">
+        <v>UAT24</v>
       </c>
       <c r="K12" t="str">
-        <v>Loan Maintenance shold be clicked</v>
+        <v xml:space="preserve">Short namae should be filled </v>
       </c>
     </row>
     <row r="13">
@@ -776,22 +794,22 @@
         <v>YES</v>
       </c>
       <c r="F13" t="str">
-        <v>TS001TC001BR012</v>
+        <v>TS001TC002TSP007</v>
       </c>
       <c r="G13" t="str">
-        <v>Enter Account ID</v>
+        <v>enter customer category</v>
       </c>
       <c r="H13" t="str">
         <v>fill</v>
       </c>
       <c r="I13" t="str">
-        <v>Account ID</v>
+        <v>Customer Category</v>
       </c>
       <c r="J13" t="str">
-        <v>2000640070000010</v>
+        <v>INDIVIDUAL</v>
       </c>
       <c r="K13" t="str">
-        <v>Account ID should be entered</v>
+        <v>Customer category  should be filled</v>
       </c>
     </row>
     <row r="14">
@@ -799,24 +817,601 @@
         <v>YES</v>
       </c>
       <c r="F14" t="str">
-        <v>TS001TC001BR013</v>
+        <v>TS001TC002TSP008</v>
       </c>
       <c r="G14" t="str">
-        <v>Click View</v>
+        <v>enter address 1</v>
       </c>
       <c r="H14" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Address 1</v>
+      </c>
+      <c r="J14" t="str">
+        <v>MASERU,LESOTHO</v>
+      </c>
+      <c r="K14" t="str">
+        <v xml:space="preserve">Address1 should be filled </v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F15" t="str">
+        <v>TS001TC002TSP009</v>
+      </c>
+      <c r="G15" t="str">
+        <v>enter country</v>
+      </c>
+      <c r="H15" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Country</v>
+      </c>
+      <c r="J15" t="str">
+        <v>LS</v>
+      </c>
+      <c r="K15" t="str">
+        <v xml:space="preserve">Country should be filled </v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F16" t="str">
+        <v>TS001TC002TSP010</v>
+      </c>
+      <c r="G16" t="str">
+        <v>enter nationality</v>
+      </c>
+      <c r="H16" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Nationality</v>
+      </c>
+      <c r="J16" t="str">
+        <v>LS</v>
+      </c>
+      <c r="K16" t="str">
+        <v xml:space="preserve">Nationality should be filled </v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F17" t="str">
+        <v>TS001TC002TSP011</v>
+      </c>
+      <c r="G17" t="str">
+        <v>select gender</v>
+      </c>
+      <c r="H17" t="str">
         <v>click</v>
       </c>
-      <c r="I14" t="str">
-        <v>View</v>
-      </c>
-      <c r="K14" t="str">
-        <v>View should be clicked</v>
+      <c r="I17" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="J17" t="str">
+        <v>MALE</v>
+      </c>
+      <c r="K17" t="str">
+        <v xml:space="preserve">Gender should clicked </v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F18" t="str">
+        <v>TS001TC002TSP012</v>
+      </c>
+      <c r="G18" t="str">
+        <v>enter date of birth</v>
+      </c>
+      <c r="H18" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Date of Birth</v>
+      </c>
+      <c r="J18" t="str">
+        <v>2001-11-12</v>
+      </c>
+      <c r="K18" t="str">
+        <v xml:space="preserve">DOB should be entered </v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F19" t="str">
+        <v>TS001TC002TSP013</v>
+      </c>
+      <c r="G19" t="str">
+        <v>select language</v>
+      </c>
+      <c r="H19" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Language</v>
+      </c>
+      <c r="J19" t="str">
+        <v>ENG</v>
+      </c>
+      <c r="K19" t="str">
+        <v xml:space="preserve">Language should be entered </v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F20" t="str">
+        <v>TS001TC002TSP014</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Click the additional button</v>
+      </c>
+      <c r="H20" t="str">
+        <v>click</v>
+      </c>
+      <c r="I20" t="str">
+        <v>Additional</v>
+      </c>
+      <c r="K20" t="str">
+        <v xml:space="preserve">Additional should be clicked </v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F21" t="str">
+        <v>TS001TC002TSP015</v>
+      </c>
+      <c r="G21" t="str">
+        <v>enter location</v>
+      </c>
+      <c r="H21" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Location</v>
+      </c>
+      <c r="J21" t="str">
+        <v>MSU</v>
+      </c>
+      <c r="K21" t="str">
+        <v xml:space="preserve">Location should be filled </v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F22" t="str">
+        <v>TS001TC002TSP016</v>
+      </c>
+      <c r="G22" t="str">
+        <v>enter media</v>
+      </c>
+      <c r="H22" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I22" t="str">
+        <v>Media</v>
+      </c>
+      <c r="J22" t="str">
+        <v>RTGS</v>
+      </c>
+      <c r="K22" t="str">
+        <v xml:space="preserve">Media should be filled </v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F23" t="str">
+        <v>TS001TC002TSP017</v>
+      </c>
+      <c r="G23" t="str">
+        <v xml:space="preserve">click on save </v>
+      </c>
+      <c r="H23" t="str">
+        <v>click</v>
+      </c>
+      <c r="I23" t="str">
+        <v>Save</v>
+      </c>
+      <c r="K23" t="str">
+        <v xml:space="preserve">Save should be clicked </v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F24" t="str">
+        <v>TS001TC002TSP018</v>
+      </c>
+      <c r="G24" t="str">
+        <v xml:space="preserve">Click  accept </v>
+      </c>
+      <c r="H24" t="str">
+        <v>click</v>
+      </c>
+      <c r="I24" t="str">
+        <v>Accept</v>
+      </c>
+      <c r="K24" t="str">
+        <v xml:space="preserve">Accept should be clicked </v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F25" t="str">
+        <v>TS001TC002TSP003</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Click Enter Query</v>
+      </c>
+      <c r="H25" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I25" t="str">
+        <v>Enter Query</v>
+      </c>
+      <c r="J25" t="str">
+        <v>Enter Query</v>
+      </c>
+      <c r="K25" t="str">
+        <v xml:space="preserve">Enter Query should be clicked </v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F26" t="str">
+        <v>TS001TC002TSP004</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Enter Customer No</v>
+      </c>
+      <c r="H26" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I26" t="str">
+        <v>Customer No</v>
+      </c>
+      <c r="J26">
+        <v>10381197</v>
+      </c>
+      <c r="K26" t="str">
+        <v>Customer number should be entered</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F27" t="str">
+        <v>TS001TC002TSP005</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Enter Currency</v>
+      </c>
+      <c r="H27" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I27" t="str">
+        <v>Currency</v>
+      </c>
+      <c r="J27" t="str">
+        <v>LSL</v>
+      </c>
+      <c r="K27" t="str">
+        <v>Currency should be entered</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F28" t="str">
+        <v>TS001TC002TSP006</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Enter Account Class</v>
+      </c>
+      <c r="H28" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I28" t="str">
+        <v>Account Class</v>
+      </c>
+      <c r="J28">
+        <v>120</v>
+      </c>
+      <c r="K28" t="str">
+        <v>Account class should be entered</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F29" t="str">
+        <v>TS001TC002TSP007</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Click Fetch and the account number is displayed on screen</v>
+      </c>
+      <c r="H29" t="str">
+        <v>click</v>
+      </c>
+      <c r="I29" t="str">
+        <v>button</v>
+      </c>
+      <c r="K29" t="str">
+        <v>Fetch button should be clicked</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F30" t="str">
+        <v>TS001TC002TSP008</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Enter Location</v>
+      </c>
+      <c r="H30" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I30" t="str">
+        <v>Location</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" t="str">
+        <v>Location should be entered</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F31" t="str">
+        <v>TS001TC002TSP009</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Enter Media</v>
+      </c>
+      <c r="H31" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I31" t="str">
+        <v>Media</v>
+      </c>
+      <c r="J31" t="str">
+        <v>RTGS</v>
+      </c>
+      <c r="K31" t="str">
+        <v>Media should be entered</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F32" t="str">
+        <v>TS001TC002TSP010</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Select MIS tab and enter Pool Code</v>
+      </c>
+      <c r="H32" t="str">
+        <v>fill</v>
+      </c>
+      <c r="I32" t="str">
+        <v>Pool Code</v>
+      </c>
+      <c r="J32" t="str">
+        <v>DFLTPOOL</v>
+      </c>
+      <c r="K32" t="str">
+        <v xml:space="preserve">Pool code should be entered </v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F33" t="str">
+        <v>TS001TC002TSP011</v>
+      </c>
+      <c r="G33" t="str">
+        <v xml:space="preserve">Click on save and select accept </v>
+      </c>
+      <c r="H33" t="str">
+        <v>click</v>
+      </c>
+      <c r="I33" t="str">
+        <v>button</v>
+      </c>
+      <c r="K33" t="str">
+        <v xml:space="preserve">Save and Select accept should be clicked </v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>NO</v>
+      </c>
+      <c r="B34" t="str">
+        <v>TS002</v>
+      </c>
+      <c r="D34" t="str">
+        <v>TS111TC001</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Flipkart</v>
+      </c>
+      <c r="F34" t="str">
+        <v>TS111TC001TSP001</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Open the url</v>
+      </c>
+      <c r="H34" t="str">
+        <v>OPEN_URL</v>
+      </c>
+      <c r="I34" t="str">
+        <v>https://www.flipkart.com/</v>
+      </c>
+      <c r="J34" t="str">
+        <v>https://www.flipkart.com/</v>
+      </c>
+      <c r="K34" t="str">
+        <v>URL should be opened</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F35" t="str">
+        <v>TS111TC001TSP002</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Click Login</v>
+      </c>
+      <c r="H35" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I35" t="str">
+        <v>Login</v>
+      </c>
+      <c r="K35" t="str">
+        <v>Login should be clicked</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F36" t="str">
+        <v>TS111TC001TSP003</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Click Men</v>
+      </c>
+      <c r="H36" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I36" t="str">
+        <v>Men</v>
+      </c>
+      <c r="K36" t="str">
+        <v>Men should be clicked</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F37" t="str">
+        <v>TS111TC001TSP004</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Click Running Shoes</v>
+      </c>
+      <c r="H37" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I37" t="str">
+        <v>Running Shoes</v>
+      </c>
+      <c r="K37" t="str">
+        <v>Running shoes should be clicked</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F38" t="str">
+        <v>TS111TC001TSP005</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Click COLOR</v>
+      </c>
+      <c r="H38" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I38" t="str">
+        <v>COLOR</v>
+      </c>
+      <c r="K38" t="str">
+        <v xml:space="preserve">COLOR should be clicked </v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F39" t="str">
+        <v>TS111TC001TSP006</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Click Blue</v>
+      </c>
+      <c r="H39" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I39" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="K39" t="str">
+        <v>Blue should be selected</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F40" t="str">
+        <v>TS111TC001TSP007</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Click BestSeller</v>
+      </c>
+      <c r="H40" t="str">
+        <v>Click</v>
+      </c>
+      <c r="I40" t="str">
+        <v>BestSeller</v>
+      </c>
+      <c r="K40" t="str">
+        <v xml:space="preserve">Best seller product should be clicked </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix automation hanging issue - reduce waitForPageReady timeouts and make page readiness non-blocking
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -717,10 +717,10 @@
         <v>Failed to click: New</v>
       </c>
       <c r="O9" t="str">
-        <v>screenshots/STEP_8.png</v>
+        <v/>
       </c>
       <c r="P9" t="str">
-        <v>page_sources/STEP_8_source.html</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -742,6 +742,21 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
+      <c r="L10" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M10" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N10" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -765,6 +780,21 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
+      <c r="L11" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M11" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N11" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -788,6 +818,21 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
+      <c r="L12" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M12" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N12" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -811,6 +856,21 @@
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
       </c>
+      <c r="L13" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M13" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N13" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -834,6 +894,21 @@
       <c r="K14" t="str">
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
+      <c r="L14" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M14" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N14" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -857,6 +932,21 @@
       <c r="K15" t="str">
         <v xml:space="preserve">Country should be filled </v>
       </c>
+      <c r="L15" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M15" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N15" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -880,6 +970,21 @@
       <c r="K16" t="str">
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
+      <c r="L16" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M16" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N16" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -903,6 +1008,21 @@
       <c r="K17" t="str">
         <v xml:space="preserve">Gender should clicked </v>
       </c>
+      <c r="L17" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M17" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N17" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -926,6 +1046,21 @@
       <c r="K18" t="str">
         <v xml:space="preserve">DOB should be entered </v>
       </c>
+      <c r="L18" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M18" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N18" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -949,6 +1084,21 @@
       <c r="K19" t="str">
         <v xml:space="preserve">Language should be entered </v>
       </c>
+      <c r="L19" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M19" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N19" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -969,6 +1119,21 @@
       <c r="K20" t="str">
         <v xml:space="preserve">Additional should be clicked </v>
       </c>
+      <c r="L20" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M20" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N20" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -992,6 +1157,21 @@
       <c r="K21" t="str">
         <v xml:space="preserve">Location should be filled </v>
       </c>
+      <c r="L21" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M21" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N21" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1015,6 +1195,21 @@
       <c r="K22" t="str">
         <v xml:space="preserve">Media should be filled </v>
       </c>
+      <c r="L22" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M22" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N22" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1035,6 +1230,21 @@
       <c r="K23" t="str">
         <v xml:space="preserve">Save should be clicked </v>
       </c>
+      <c r="L23" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M23" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N23" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1055,6 +1265,21 @@
       <c r="K24" t="str">
         <v xml:space="preserve">Accept should be clicked </v>
       </c>
+      <c r="L24" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M24" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N24" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1075,6 +1300,12 @@
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>
       </c>
+      <c r="L25" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M25" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1098,6 +1329,12 @@
       <c r="K26" t="str">
         <v>Customer number should be entered</v>
       </c>
+      <c r="L26" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M26" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1121,6 +1358,12 @@
       <c r="K27" t="str">
         <v>Currency should be entered</v>
       </c>
+      <c r="L27" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M27" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1144,6 +1387,12 @@
       <c r="K28" t="str">
         <v>Account class should be entered</v>
       </c>
+      <c r="L28" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M28" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1164,6 +1413,12 @@
       <c r="K29" t="str">
         <v>Fetch button should be clicked</v>
       </c>
+      <c r="L29" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M29" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1187,6 +1442,12 @@
       <c r="K30" t="str">
         <v>Location should be entered</v>
       </c>
+      <c r="L30" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M30" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1210,6 +1471,12 @@
       <c r="K31" t="str">
         <v>Media should be entered</v>
       </c>
+      <c r="L31" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M31" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1233,6 +1500,12 @@
       <c r="K32" t="str">
         <v xml:space="preserve">Pool code should be entered </v>
       </c>
+      <c r="L32" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M32" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1253,6 +1526,12 @@
       <c r="K33" t="str">
         <v xml:space="preserve">Save and Select accept should be clicked </v>
       </c>
+      <c r="L33" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M33" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1285,6 +1564,12 @@
       <c r="K34" t="str">
         <v>URL should be opened</v>
       </c>
+      <c r="L34" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M34" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1305,6 +1590,12 @@
       <c r="K35" t="str">
         <v>Login should be clicked</v>
       </c>
+      <c r="L35" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M35" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1325,6 +1616,12 @@
       <c r="K36" t="str">
         <v>Men should be clicked</v>
       </c>
+      <c r="L36" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M36" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1345,6 +1642,12 @@
       <c r="K37" t="str">
         <v>Running shoes should be clicked</v>
       </c>
+      <c r="L37" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M37" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1365,6 +1668,12 @@
       <c r="K38" t="str">
         <v xml:space="preserve">COLOR should be clicked </v>
       </c>
+      <c r="L38" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M38" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1385,6 +1694,12 @@
       <c r="K39" t="str">
         <v>Blue should be selected</v>
       </c>
+      <c r="L39" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M39" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1404,6 +1719,12 @@
       </c>
       <c r="K40" t="str">
         <v xml:space="preserve">Best seller product should be clicked </v>
+      </c>
+      <c r="L40" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M40" t="str">
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add overlay window and modal detection support
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -487,19 +487,19 @@
         <v xml:space="preserve">URL is opened </v>
       </c>
       <c r="L2" t="str">
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="M2" t="str">
+        <v>Cannot read properties of null (reading 'isClosed')</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Cannot read properties of null (reading 'isClosed')</v>
+      </c>
+      <c r="O2" t="str">
         <v/>
       </c>
-      <c r="N2" t="str">
-        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
-      </c>
-      <c r="O2" t="str">
-        <v>screenshots/STEP_1.png</v>
-      </c>
       <c r="P2" t="str">
-        <v>page_sources/STEP_1_source.html</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -524,12 +524,6 @@
       <c r="K3" t="str">
         <v>username should be entered</v>
       </c>
-      <c r="L3" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M3" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -553,12 +547,6 @@
       <c r="K4" t="str">
         <v>password should be entered</v>
       </c>
-      <c r="L4" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M4" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -579,12 +567,6 @@
       <c r="K5" t="str">
         <v>Sign in button should be clicked</v>
       </c>
-      <c r="L5" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M5" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -602,12 +584,6 @@
       <c r="I6" t="str">
         <v>Ok</v>
       </c>
-      <c r="L6" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M6" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -637,21 +613,6 @@
       <c r="K7" t="str">
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
-      <c r="L7" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M7" t="str">
-        <v/>
-      </c>
-      <c r="N7" t="str">
-        <v>Filled: Function Id</v>
-      </c>
-      <c r="O7" t="str">
-        <v>screenshots/STEP_6.png</v>
-      </c>
-      <c r="P7" t="str">
-        <v>page_sources/STEP_6_source.html</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -672,21 +633,6 @@
       <c r="K8" t="str">
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
-      <c r="L8" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <v>Clicked: Go</v>
-      </c>
-      <c r="O8" t="str">
-        <v>screenshots/STEP_7.png</v>
-      </c>
-      <c r="P8" t="str">
-        <v>page_sources/STEP_7_source.html</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -706,21 +652,6 @@
       </c>
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
-      </c>
-      <c r="L9" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M9" t="str">
-        <v>Could not click element</v>
-      </c>
-      <c r="N9" t="str">
-        <v>Failed to click: New</v>
-      </c>
-      <c r="O9" t="str">
-        <v/>
-      </c>
-      <c r="P9" t="str">
-        <v/>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Optimization: Reduce excessive wait times for faster target-not-found detection
- Reduce dynamic element polling from 200ms to 100ms per check
- Reduce MutationObserver timeout from 500ms to 200ms
- Reduce default waitForDynamicElement timeout from 5000ms to 2000ms
- Reduce wait between retry attempts from 1500ms to 500ms
- Reduce advancedElementSearch wait from 1000ms to 300ms
- Reduce subwindow load wait from 800ms to 300ms
- Reduce per-frame wait time from 150ms to 50ms
- Reduce post-action waits from 800ms to 300ms
- Reduce iframe fill wait from 500ms to 200ms

This allows the assistant to fail fast when targets are not found and proceed immediately to the next test step instead of wasting time waiting.
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -454,7 +454,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="B2" t="str">
         <v>TS001</v>
@@ -487,19 +487,10 @@
         <v xml:space="preserve">URL is opened </v>
       </c>
       <c r="L2" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M2" t="str">
-        <v/>
-      </c>
-      <c r="N2" t="str">
-        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
-      </c>
-      <c r="O2" t="str">
-        <v>screenshots/STEP_1.png</v>
-      </c>
-      <c r="P2" t="str">
-        <v>page_sources/STEP_1_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="3">
@@ -611,7 +602,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="D7" t="str">
         <v>TS001TC002</v>
@@ -638,24 +629,15 @@
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
       <c r="L7" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M7" t="str">
-        <v/>
-      </c>
-      <c r="N7" t="str">
-        <v>Filled: Function Id</v>
-      </c>
-      <c r="O7" t="str">
-        <v>screenshots/STEP_6.png</v>
-      </c>
-      <c r="P7" t="str">
-        <v>page_sources/STEP_6_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F8" t="str">
         <v>TS001TC002TSP002</v>
@@ -673,24 +655,15 @@
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
       <c r="L8" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <v>Clicked: Go</v>
-      </c>
-      <c r="O8" t="str">
-        <v>screenshots/STEP_7.png</v>
-      </c>
-      <c r="P8" t="str">
-        <v>page_sources/STEP_7_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F9" t="str">
         <v>TS001TC002TSP003</v>
@@ -708,24 +681,15 @@
         <v xml:space="preserve">New should be clicked </v>
       </c>
       <c r="L9" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
-        <v>Clicked: New</v>
-      </c>
-      <c r="O9" t="str">
-        <v>screenshots/STEP_8.png</v>
-      </c>
-      <c r="P9" t="str">
-        <v>page_sources/STEP_8_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F10" t="str">
         <v>TS001TC002TSP004</v>
@@ -743,24 +707,15 @@
         <v>P should be clicked and Customer No should be generated</v>
       </c>
       <c r="L10" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M10" t="str">
-        <v/>
-      </c>
-      <c r="N10" t="str">
-        <v>Clicked: P</v>
-      </c>
-      <c r="O10" t="str">
-        <v>screenshots/STEP_9.png</v>
-      </c>
-      <c r="P10" t="str">
-        <v>page_sources/STEP_9_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F11" t="str">
         <v>TS001TC002TSP005</v>
@@ -781,24 +736,15 @@
         <v xml:space="preserve">First name should be filled </v>
       </c>
       <c r="L11" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M11" t="str">
-        <v/>
-      </c>
-      <c r="N11" t="str">
-        <v>Filled: Full Name</v>
-      </c>
-      <c r="O11" t="str">
-        <v>screenshots/STEP_10.png</v>
-      </c>
-      <c r="P11" t="str">
-        <v>page_sources/STEP_10_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F12" t="str">
         <v>TS001TC002TSP006</v>
@@ -819,24 +765,15 @@
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
       <c r="L12" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M12" t="str">
-        <v/>
-      </c>
-      <c r="N12" t="str">
-        <v>Filled: Short Name</v>
-      </c>
-      <c r="O12" t="str">
-        <v>screenshots/STEP_11.png</v>
-      </c>
-      <c r="P12" t="str">
-        <v>page_sources/STEP_11_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F13" t="str">
         <v>TS001TC002TSP007</v>
@@ -857,24 +794,15 @@
         <v>Customer category  should be filled</v>
       </c>
       <c r="L13" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M13" t="str">
-        <v/>
-      </c>
-      <c r="N13" t="str">
-        <v>Filled: Customer Category</v>
-      </c>
-      <c r="O13" t="str">
-        <v>screenshots/STEP_12.png</v>
-      </c>
-      <c r="P13" t="str">
-        <v>page_sources/STEP_12_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F14" t="str">
         <v>TS001TC002TSP008</v>
@@ -895,24 +823,15 @@
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
       <c r="L14" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M14" t="str">
-        <v/>
-      </c>
-      <c r="N14" t="str">
-        <v>Filled: Address 1</v>
-      </c>
-      <c r="O14" t="str">
-        <v>screenshots/STEP_13.png</v>
-      </c>
-      <c r="P14" t="str">
-        <v>page_sources/STEP_13_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F15" t="str">
         <v>TS001TC002TSP009</v>
@@ -933,24 +852,15 @@
         <v xml:space="preserve">Country should be filled </v>
       </c>
       <c r="L15" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M15" t="str">
-        <v/>
-      </c>
-      <c r="N15" t="str">
-        <v>Filled: Country</v>
-      </c>
-      <c r="O15" t="str">
-        <v>screenshots/STEP_14.png</v>
-      </c>
-      <c r="P15" t="str">
-        <v>page_sources/STEP_14_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F16" t="str">
         <v>TS001TC002TSP010</v>
@@ -971,24 +881,15 @@
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
       <c r="L16" t="str">
-        <v>PASS</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M16" t="str">
-        <v/>
-      </c>
-      <c r="N16" t="str">
-        <v>Filled: Nationality</v>
-      </c>
-      <c r="O16" t="str">
-        <v>screenshots/STEP_15.png</v>
-      </c>
-      <c r="P16" t="str">
-        <v>page_sources/STEP_15_source.html</v>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F17" t="str">
         <v>TS001TC002TSP011</v>
@@ -1009,24 +910,15 @@
         <v xml:space="preserve">Gender should clicked </v>
       </c>
       <c r="L17" t="str">
-        <v>FAIL</v>
+        <v>SKIPPED</v>
       </c>
       <c r="M17" t="str">
-        <v>Could not click element</v>
-      </c>
-      <c r="N17" t="str">
-        <v>Failed to click: Gender</v>
-      </c>
-      <c r="O17" t="str">
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <v/>
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F18" t="str">
         <v>TS001TC002TSP012</v>
@@ -1046,10 +938,16 @@
       <c r="K18" t="str">
         <v xml:space="preserve">DOB should be entered </v>
       </c>
+      <c r="L18" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M18" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F19" t="str">
         <v>TS001TC002TSP013</v>
@@ -1069,10 +967,16 @@
       <c r="K19" t="str">
         <v xml:space="preserve">Language should be entered </v>
       </c>
+      <c r="L19" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M19" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F20" t="str">
         <v>TS001TC002TSP014</v>
@@ -1089,10 +993,16 @@
       <c r="K20" t="str">
         <v xml:space="preserve">Additional should be clicked </v>
       </c>
+      <c r="L20" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M20" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F21" t="str">
         <v>TS001TC002TSP015</v>
@@ -1112,10 +1022,16 @@
       <c r="K21" t="str">
         <v xml:space="preserve">Location should be filled </v>
       </c>
+      <c r="L21" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M21" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F22" t="str">
         <v>TS001TC002TSP016</v>
@@ -1135,10 +1051,16 @@
       <c r="K22" t="str">
         <v xml:space="preserve">Media should be filled </v>
       </c>
+      <c r="L22" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M22" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F23" t="str">
         <v>TS001TC002TSP017</v>
@@ -1155,10 +1077,16 @@
       <c r="K23" t="str">
         <v xml:space="preserve">Save should be clicked </v>
       </c>
+      <c r="L23" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M23" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F24" t="str">
         <v>TS001TC002TSP018</v>
@@ -1175,6 +1103,12 @@
       <c r="K24" t="str">
         <v xml:space="preserve">Accept should be clicked </v>
       </c>
+      <c r="L24" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M24" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1195,6 +1129,12 @@
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>
       </c>
+      <c r="L25" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M25" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1218,6 +1158,12 @@
       <c r="K26" t="str">
         <v>Customer number should be entered</v>
       </c>
+      <c r="L26" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M26" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1241,6 +1187,12 @@
       <c r="K27" t="str">
         <v>Currency should be entered</v>
       </c>
+      <c r="L27" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M27" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1264,6 +1216,12 @@
       <c r="K28" t="str">
         <v>Account class should be entered</v>
       </c>
+      <c r="L28" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M28" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1284,6 +1242,12 @@
       <c r="K29" t="str">
         <v>Fetch button should be clicked</v>
       </c>
+      <c r="L29" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M29" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1307,6 +1271,12 @@
       <c r="K30" t="str">
         <v>Location should be entered</v>
       </c>
+      <c r="L30" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M30" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1330,6 +1300,12 @@
       <c r="K31" t="str">
         <v>Media should be entered</v>
       </c>
+      <c r="L31" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M31" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1353,6 +1329,12 @@
       <c r="K32" t="str">
         <v xml:space="preserve">Pool code should be entered </v>
       </c>
+      <c r="L32" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M32" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1373,10 +1355,16 @@
       <c r="K33" t="str">
         <v xml:space="preserve">Save and Select accept should be clicked </v>
       </c>
+      <c r="L33" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M33" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B34" t="str">
         <v>TS002</v>
@@ -1405,10 +1393,25 @@
       <c r="K34" t="str">
         <v>URL should be opened</v>
       </c>
+      <c r="L34" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M34" t="str">
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <v>Opened: https://www.flipkart.com/</v>
+      </c>
+      <c r="O34" t="str">
+        <v>screenshots/STEP_33.png</v>
+      </c>
+      <c r="P34" t="str">
+        <v>page_sources/STEP_33_source.html</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F35" t="str">
         <v>TS111TC001TSP002</v>
@@ -1425,10 +1428,25 @@
       <c r="K35" t="str">
         <v>Login should be clicked</v>
       </c>
+      <c r="L35" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <v>Clicked: Login</v>
+      </c>
+      <c r="O35" t="str">
+        <v>screenshots/STEP_34.png</v>
+      </c>
+      <c r="P35" t="str">
+        <v>page_sources/STEP_34_source.html</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F36" t="str">
         <v>TS111TC001TSP003</v>
@@ -1445,10 +1463,25 @@
       <c r="K36" t="str">
         <v>Men should be clicked</v>
       </c>
+      <c r="L36" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M36" t="str">
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <v>Clicked: Men</v>
+      </c>
+      <c r="O36" t="str">
+        <v>screenshots/STEP_35.png</v>
+      </c>
+      <c r="P36" t="str">
+        <v>page_sources/STEP_35_source.html</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F37" t="str">
         <v>TS111TC001TSP004</v>
@@ -1465,10 +1498,25 @@
       <c r="K37" t="str">
         <v>Running shoes should be clicked</v>
       </c>
+      <c r="L37" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+      <c r="N37" t="str">
+        <v>Clicked: Running Shoes</v>
+      </c>
+      <c r="O37" t="str">
+        <v>screenshots/STEP_36.png</v>
+      </c>
+      <c r="P37" t="str">
+        <v>page_sources/STEP_36_source.html</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F38" t="str">
         <v>TS111TC001TSP005</v>
@@ -1485,10 +1533,25 @@
       <c r="K38" t="str">
         <v xml:space="preserve">COLOR should be clicked </v>
       </c>
+      <c r="L38" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M38" t="str">
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <v>Clicked: COLOR</v>
+      </c>
+      <c r="O38" t="str">
+        <v>screenshots/STEP_37.png</v>
+      </c>
+      <c r="P38" t="str">
+        <v>page_sources/STEP_37_source.html</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F39" t="str">
         <v>TS111TC001TSP006</v>
@@ -1505,10 +1568,25 @@
       <c r="K39" t="str">
         <v>Blue should be selected</v>
       </c>
+      <c r="L39" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M39" t="str">
+        <v>Could not click element</v>
+      </c>
+      <c r="N39" t="str">
+        <v>Failed to click: Blue</v>
+      </c>
+      <c r="O39" t="str">
+        <v>screenshots/STEP_38.png</v>
+      </c>
+      <c r="P39" t="str">
+        <v>page_sources/STEP_38_source.html</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="F40" t="str">
         <v>TS111TC001TSP007</v>
@@ -1524,6 +1602,21 @@
       </c>
       <c r="K40" t="str">
         <v xml:space="preserve">Best seller product should be clicked </v>
+      </c>
+      <c r="L40" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M40" t="str">
+        <v>Could not click element</v>
+      </c>
+      <c r="N40" t="str">
+        <v>Failed to click: BestSeller</v>
+      </c>
+      <c r="O40" t="str">
+        <v>screenshots/STEP_39.png</v>
+      </c>
+      <c r="P40" t="str">
+        <v>page_sources/STEP_39_source.html</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD OVERLAY SEARCH: Customer Maintenance and overlaid forms now searchable FIRST - Priority 0 for modals/dialogs/overlays rendered on main page
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -487,19 +487,19 @@
         <v xml:space="preserve">URL is opened </v>
       </c>
       <c r="L2" t="str">
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="M2" t="str">
-        <v>Cannot read properties of null (reading 'isClosed')</v>
+        <v/>
       </c>
       <c r="N2" t="str">
-        <v>Cannot read properties of null (reading 'isClosed')</v>
+        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
       </c>
       <c r="O2" t="str">
-        <v/>
+        <v>screenshots/STEP_1.png</v>
       </c>
       <c r="P2" t="str">
-        <v/>
+        <v>page_sources/STEP_1_source.html</v>
       </c>
     </row>
     <row r="3">
@@ -524,6 +524,12 @@
       <c r="K3" t="str">
         <v>username should be entered</v>
       </c>
+      <c r="L3" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M3" t="str">
+        <v>TO BE EXECUTED = "NO" (not YES)</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -547,6 +553,12 @@
       <c r="K4" t="str">
         <v>password should be entered</v>
       </c>
+      <c r="L4" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M4" t="str">
+        <v>TO BE EXECUTED = "NO" (not YES)</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -567,6 +579,12 @@
       <c r="K5" t="str">
         <v>Sign in button should be clicked</v>
       </c>
+      <c r="L5" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M5" t="str">
+        <v>TO BE EXECUTED = "NO" (not YES)</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -584,6 +602,12 @@
       <c r="I6" t="str">
         <v>Ok</v>
       </c>
+      <c r="L6" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M6" t="str">
+        <v>TO BE EXECUTED = "NO" (not YES)</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -613,6 +637,21 @@
       <c r="K7" t="str">
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
+      <c r="L7" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v>Filled: Function Id</v>
+      </c>
+      <c r="O7" t="str">
+        <v>screenshots/STEP_6.png</v>
+      </c>
+      <c r="P7" t="str">
+        <v>page_sources/STEP_6_source.html</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -633,6 +672,21 @@
       <c r="K8" t="str">
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
+      <c r="L8" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v>Clicked: Go</v>
+      </c>
+      <c r="O8" t="str">
+        <v>screenshots/STEP_7.png</v>
+      </c>
+      <c r="P8" t="str">
+        <v>page_sources/STEP_7_source.html</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -653,6 +707,21 @@
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
       </c>
+      <c r="L9" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v>Clicked: New</v>
+      </c>
+      <c r="O9" t="str">
+        <v>screenshots/STEP_8.png</v>
+      </c>
+      <c r="P9" t="str">
+        <v>page_sources/STEP_8_source.html</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -673,6 +742,21 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
+      <c r="L10" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v>Clicked: P</v>
+      </c>
+      <c r="O10" t="str">
+        <v>screenshots/STEP_9.png</v>
+      </c>
+      <c r="P10" t="str">
+        <v>page_sources/STEP_9_source.html</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -696,6 +780,21 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
+      <c r="L11" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v>Filled: Full Name</v>
+      </c>
+      <c r="O11" t="str">
+        <v>screenshots/STEP_10.png</v>
+      </c>
+      <c r="P11" t="str">
+        <v>page_sources/STEP_10_source.html</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -719,6 +818,21 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
+      <c r="L12" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v>Filled: Short Name</v>
+      </c>
+      <c r="O12" t="str">
+        <v>screenshots/STEP_11.png</v>
+      </c>
+      <c r="P12" t="str">
+        <v>page_sources/STEP_11_source.html</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -741,6 +855,21 @@
       </c>
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
+      </c>
+      <c r="L13" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v>Filled: Customer Category</v>
+      </c>
+      <c r="O13" t="str">
+        <v>screenshots/STEP_12.png</v>
+      </c>
+      <c r="P13" t="str">
+        <v>page_sources/STEP_12_source.html</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
FIX SEARCH PRIORITY: Search main page FIRST, overlays LAST - prevents clicking wrong elements on main page
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -638,19 +638,19 @@
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
       <c r="L7" t="str">
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="M7" t="str">
-        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+        <v/>
       </c>
       <c r="N7" t="str">
-        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+        <v>Filled: Function Id</v>
       </c>
       <c r="O7" t="str">
-        <v/>
+        <v>screenshots/STEP_6.png</v>
       </c>
       <c r="P7" t="str">
-        <v/>
+        <v>page_sources/STEP_6_source.html</v>
       </c>
     </row>
     <row r="8">
@@ -672,6 +672,21 @@
       <c r="K8" t="str">
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
+      <c r="L8" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v>Clicked: Go</v>
+      </c>
+      <c r="O8" t="str">
+        <v>screenshots/STEP_7.png</v>
+      </c>
+      <c r="P8" t="str">
+        <v>page_sources/STEP_7_source.html</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -692,6 +707,21 @@
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
       </c>
+      <c r="L9" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v>Clicked: New</v>
+      </c>
+      <c r="O9" t="str">
+        <v>screenshots/STEP_8.png</v>
+      </c>
+      <c r="P9" t="str">
+        <v>page_sources/STEP_8_source.html</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -712,6 +742,21 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
+      <c r="L10" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v>Clicked: P</v>
+      </c>
+      <c r="O10" t="str">
+        <v>screenshots/STEP_9.png</v>
+      </c>
+      <c r="P10" t="str">
+        <v>page_sources/STEP_9_source.html</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -735,6 +780,21 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
+      <c r="L11" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v>Filled: Full Name</v>
+      </c>
+      <c r="O11" t="str">
+        <v>screenshots/STEP_10.png</v>
+      </c>
+      <c r="P11" t="str">
+        <v>page_sources/STEP_10_source.html</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -758,6 +818,21 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
+      <c r="L12" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v>Filled: Short Name</v>
+      </c>
+      <c r="O12" t="str">
+        <v>screenshots/STEP_11.png</v>
+      </c>
+      <c r="P12" t="str">
+        <v>page_sources/STEP_11_source.html</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -780,6 +855,21 @@
       </c>
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
+      </c>
+      <c r="L13" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v>Filled: Customer Category</v>
+      </c>
+      <c r="O13" t="str">
+        <v>screenshots/STEP_12.png</v>
+      </c>
+      <c r="P13" t="str">
+        <v>page_sources/STEP_12_source.html</v>
       </c>
     </row>
     <row r="14">

</xml_diff>